<commit_message>
:tada: | Search item in database
</commit_message>
<xml_diff>
--- a/judite/data/xlsx/data.xlsx
+++ b/judite/data/xlsx/data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateus\projects\judite\judite\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E128CCEA-38D3-4790-81DA-22978E3BBE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E77AAC-F813-4CFF-B2B9-EC45CD9189DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DC77D82C-3D1A-4928-B2F9-AAED9DFD6818}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="livros" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -404,7 +404,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>